<commit_message>
Add verbs Check List A-B and missing some facts
</commit_message>
<xml_diff>
--- a/Verbs list.xlsx
+++ b/Verbs list.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="332">
   <si>
     <t>catch</t>
   </si>
@@ -674,9 +674,6 @@
     <t>frozen</t>
   </si>
   <si>
-    <t>froze</t>
-  </si>
-  <si>
     <t>wake</t>
   </si>
   <si>
@@ -837,6 +834,192 @@
   </si>
   <si>
     <t>Fallen</t>
+  </si>
+  <si>
+    <t>know</t>
+  </si>
+  <si>
+    <t>knew</t>
+  </si>
+  <si>
+    <t>known</t>
+  </si>
+  <si>
+    <t>grow</t>
+  </si>
+  <si>
+    <t>grew</t>
+  </si>
+  <si>
+    <t>grown</t>
+  </si>
+  <si>
+    <t>blow</t>
+  </si>
+  <si>
+    <t>blew</t>
+  </si>
+  <si>
+    <t>blown</t>
+  </si>
+  <si>
+    <t>throw</t>
+  </si>
+  <si>
+    <t>threw</t>
+  </si>
+  <si>
+    <t>fly</t>
+  </si>
+  <si>
+    <t>flew</t>
+  </si>
+  <si>
+    <t>flown</t>
+  </si>
+  <si>
+    <t>draw</t>
+  </si>
+  <si>
+    <t>drew</t>
+  </si>
+  <si>
+    <t>drawn</t>
+  </si>
+  <si>
+    <t>withdraw</t>
+  </si>
+  <si>
+    <t>withdrew</t>
+  </si>
+  <si>
+    <t>withdrawn</t>
+  </si>
+  <si>
+    <t>come</t>
+  </si>
+  <si>
+    <t>came</t>
+  </si>
+  <si>
+    <t>become</t>
+  </si>
+  <si>
+    <t>became</t>
+  </si>
+  <si>
+    <t>overcome</t>
+  </si>
+  <si>
+    <t>overcame</t>
+  </si>
+  <si>
+    <t>lie</t>
+  </si>
+  <si>
+    <t>lain</t>
+  </si>
+  <si>
+    <t>underlie</t>
+  </si>
+  <si>
+    <t>underlay</t>
+  </si>
+  <si>
+    <t>underlain</t>
+  </si>
+  <si>
+    <t>slay</t>
+  </si>
+  <si>
+    <t>slew</t>
+  </si>
+  <si>
+    <t>slain</t>
+  </si>
+  <si>
+    <t>be</t>
+  </si>
+  <si>
+    <t>was/were</t>
+  </si>
+  <si>
+    <t>been</t>
+  </si>
+  <si>
+    <t>see</t>
+  </si>
+  <si>
+    <t>saw</t>
+  </si>
+  <si>
+    <t>seen</t>
+  </si>
+  <si>
+    <t>foresee</t>
+  </si>
+  <si>
+    <t>foresaw</t>
+  </si>
+  <si>
+    <t>foreseen</t>
+  </si>
+  <si>
+    <t>do</t>
+  </si>
+  <si>
+    <t>did</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>go</t>
+  </si>
+  <si>
+    <t>went</t>
+  </si>
+  <si>
+    <t>gone</t>
+  </si>
+  <si>
+    <t>undergo</t>
+  </si>
+  <si>
+    <t>underwent</t>
+  </si>
+  <si>
+    <t>undergone</t>
+  </si>
+  <si>
+    <t>overdo</t>
+  </si>
+  <si>
+    <t>overdid</t>
+  </si>
+  <si>
+    <t>overdone</t>
+  </si>
+  <si>
+    <t>outdo</t>
+  </si>
+  <si>
+    <t>outdid</t>
+  </si>
+  <si>
+    <t>outdone</t>
+  </si>
+  <si>
+    <t>forego</t>
+  </si>
+  <si>
+    <t>forewent</t>
+  </si>
+  <si>
+    <t>foregone</t>
+  </si>
+  <si>
+    <t>Group B</t>
   </si>
 </sst>
 </file>
@@ -882,7 +1065,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -910,6 +1093,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -950,7 +1139,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -960,9 +1149,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -976,16 +1162,22 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1268,10 +1460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AT36"/>
+  <dimension ref="A1:AT42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27:G27"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1283,115 +1475,115 @@
     <col min="6" max="6" width="13.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="15" width="11.42578125" style="1"/>
     <col min="16" max="16" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="26" width="11.42578125" style="1"/>
-    <col min="27" max="27" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="25" width="11.42578125" style="1"/>
+    <col min="26" max="27" width="15" style="1" bestFit="1" customWidth="1"/>
     <col min="28" max="35" width="11.42578125" style="1"/>
     <col min="36" max="36" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="37" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A1" s="5"/>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
+      <c r="A1" s="4"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
     </row>
     <row r="2" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="7"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="6"/>
     </row>
     <row r="3" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="7"/>
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="6"/>
     </row>
     <row r="4" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="7"/>
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="6"/>
     </row>
     <row r="5" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="7"/>
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="6"/>
     </row>
     <row r="6" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="7"/>
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="6"/>
     </row>
     <row r="7" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="7"/>
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="6"/>
     </row>
     <row r="8" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="7"/>
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="6"/>
     </row>
     <row r="9" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
     </row>
     <row r="10" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
     </row>
     <row r="11" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
+      <c r="A11" s="10">
         <v>7</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="I11" s="4">
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="I11" s="10">
         <v>9</v>
       </c>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
-      <c r="O11" s="4"/>
-      <c r="P11" s="4"/>
-      <c r="Q11" s="4"/>
-      <c r="S11" s="4">
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="10"/>
+      <c r="Q11" s="10"/>
+      <c r="S11" s="10">
         <v>8</v>
       </c>
-      <c r="T11" s="4"/>
-      <c r="U11" s="4"/>
-      <c r="V11" s="4"/>
-      <c r="W11" s="4"/>
-      <c r="X11" s="4"/>
-      <c r="Y11" s="4"/>
-      <c r="Z11" s="4"/>
-      <c r="AB11" s="4">
+      <c r="T11" s="10"/>
+      <c r="U11" s="10"/>
+      <c r="V11" s="10"/>
+      <c r="W11" s="10"/>
+      <c r="X11" s="10"/>
+      <c r="Y11" s="10"/>
+      <c r="Z11" s="10"/>
+      <c r="AB11" s="10">
         <v>6</v>
       </c>
-      <c r="AC11" s="4"/>
-      <c r="AD11" s="4"/>
-      <c r="AE11" s="4"/>
-      <c r="AF11" s="4"/>
-      <c r="AG11" s="4"/>
-      <c r="AI11" s="4">
+      <c r="AC11" s="10"/>
+      <c r="AD11" s="10"/>
+      <c r="AE11" s="10"/>
+      <c r="AF11" s="10"/>
+      <c r="AG11" s="10"/>
+      <c r="AI11" s="10">
         <v>4</v>
       </c>
-      <c r="AJ11" s="4"/>
-      <c r="AK11" s="4"/>
-      <c r="AL11" s="4"/>
-      <c r="AN11" s="4">
+      <c r="AJ11" s="10"/>
+      <c r="AK11" s="10"/>
+      <c r="AL11" s="10"/>
+      <c r="AN11" s="10">
         <v>5</v>
       </c>
-      <c r="AO11" s="4"/>
-      <c r="AP11" s="4"/>
-      <c r="AQ11" s="4"/>
-      <c r="AR11" s="4"/>
+      <c r="AO11" s="10"/>
+      <c r="AP11" s="10"/>
+      <c r="AQ11" s="10"/>
+      <c r="AR11" s="10"/>
     </row>
     <row r="12" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
@@ -1766,59 +1958,59 @@
       </c>
     </row>
     <row r="17" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A17" s="4">
+      <c r="A17" s="10">
         <v>5</v>
       </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="G17" s="4">
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="G17" s="10">
         <v>3</v>
       </c>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="K17" s="4">
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="K17" s="10">
         <v>3</v>
       </c>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-      <c r="O17" s="4">
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
+      <c r="O17" s="10">
         <v>3</v>
       </c>
-      <c r="P17" s="4"/>
-      <c r="Q17" s="4"/>
-      <c r="S17" s="4">
+      <c r="P17" s="10"/>
+      <c r="Q17" s="10"/>
+      <c r="S17" s="10">
         <v>4</v>
       </c>
-      <c r="T17" s="4"/>
-      <c r="U17" s="4"/>
-      <c r="V17" s="4"/>
-      <c r="X17" s="4">
+      <c r="T17" s="10"/>
+      <c r="U17" s="10"/>
+      <c r="V17" s="10"/>
+      <c r="X17" s="10">
         <v>2</v>
       </c>
-      <c r="Y17" s="4"/>
-      <c r="AA17" s="4">
+      <c r="Y17" s="10"/>
+      <c r="AA17" s="10">
         <v>4</v>
       </c>
-      <c r="AB17" s="4"/>
-      <c r="AC17" s="4"/>
-      <c r="AD17" s="4"/>
-      <c r="AF17" s="4">
+      <c r="AB17" s="10"/>
+      <c r="AC17" s="10"/>
+      <c r="AD17" s="10"/>
+      <c r="AF17" s="10">
         <v>3</v>
       </c>
-      <c r="AG17" s="4"/>
-      <c r="AH17" s="4"/>
-      <c r="AJ17" s="4">
+      <c r="AG17" s="10"/>
+      <c r="AH17" s="10"/>
+      <c r="AJ17" s="10">
         <v>4</v>
       </c>
-      <c r="AK17" s="4"/>
-      <c r="AL17" s="4"/>
-      <c r="AM17" s="4"/>
-      <c r="AO17" s="4">
+      <c r="AK17" s="10"/>
+      <c r="AL17" s="10"/>
+      <c r="AM17" s="10"/>
+      <c r="AO17" s="10">
         <v>2</v>
       </c>
-      <c r="AP17" s="4"/>
+      <c r="AP17" s="10"/>
     </row>
     <row r="18" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
@@ -2151,77 +2343,77 @@
       </c>
     </row>
     <row r="22" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
+      <c r="A22" s="7" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="23" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A23" s="9">
+      <c r="A23" s="11">
         <f>SUM(A11,A17,G17,I11,K17,O17,S17,S11,X17,AB11,AI11:AL11,AF17,AJ17,AN11,AO17,AA17)</f>
         <v>72</v>
       </c>
     </row>
     <row r="24" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A24" s="9"/>
+      <c r="A24" s="11"/>
     </row>
     <row r="25" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A25" s="9"/>
+      <c r="A25" s="11"/>
     </row>
     <row r="27" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A27" s="10">
+      <c r="A27" s="12">
         <v>7</v>
       </c>
-      <c r="B27" s="10"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
-      <c r="I27" s="11">
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="I27" s="8">
         <v>10</v>
       </c>
-      <c r="J27" s="11"/>
-      <c r="K27" s="11"/>
-      <c r="L27" s="11"/>
-      <c r="M27" s="11"/>
-      <c r="N27" s="11"/>
-      <c r="O27" s="11"/>
-      <c r="P27" s="11"/>
-      <c r="Q27" s="11"/>
-      <c r="R27" s="11"/>
-      <c r="T27" s="11">
-        <v>8</v>
-      </c>
-      <c r="U27" s="11"/>
-      <c r="V27" s="11"/>
-      <c r="W27" s="11"/>
-      <c r="X27" s="11"/>
-      <c r="Y27" s="11"/>
-      <c r="Z27" s="11"/>
-      <c r="AA27" s="11"/>
-      <c r="AC27" s="11">
+      <c r="J27" s="8"/>
+      <c r="K27" s="8"/>
+      <c r="L27" s="8"/>
+      <c r="M27" s="8"/>
+      <c r="N27" s="8"/>
+      <c r="O27" s="8"/>
+      <c r="P27" s="8"/>
+      <c r="Q27" s="8"/>
+      <c r="R27" s="8"/>
+      <c r="T27" s="8">
+        <v>7</v>
+      </c>
+      <c r="U27" s="8"/>
+      <c r="V27" s="8"/>
+      <c r="W27" s="8"/>
+      <c r="X27" s="8"/>
+      <c r="Y27" s="8"/>
+      <c r="Z27" s="8"/>
+      <c r="AA27" s="6"/>
+      <c r="AC27" s="8">
         <v>4</v>
       </c>
-      <c r="AD27" s="11"/>
-      <c r="AE27" s="11"/>
-      <c r="AF27" s="11"/>
-      <c r="AH27" s="11">
+      <c r="AD27" s="8"/>
+      <c r="AE27" s="8"/>
+      <c r="AF27" s="8"/>
+      <c r="AH27" s="8">
         <v>5</v>
       </c>
-      <c r="AI27" s="11"/>
-      <c r="AJ27" s="11"/>
-      <c r="AK27" s="11"/>
-      <c r="AL27" s="11"/>
-      <c r="AN27" s="11">
+      <c r="AI27" s="8"/>
+      <c r="AJ27" s="8"/>
+      <c r="AK27" s="8"/>
+      <c r="AL27" s="8"/>
+      <c r="AN27" s="8">
         <v>2</v>
       </c>
-      <c r="AO27" s="11"/>
-      <c r="AQ27" s="11">
+      <c r="AO27" s="8"/>
+      <c r="AQ27" s="8">
         <v>4</v>
       </c>
-      <c r="AR27" s="11"/>
-      <c r="AS27" s="11"/>
-      <c r="AT27" s="11"/>
+      <c r="AR27" s="8"/>
+      <c r="AS27" s="8"/>
+      <c r="AT27" s="8"/>
     </row>
     <row r="28" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
@@ -2294,55 +2486,52 @@
         <v>213</v>
       </c>
       <c r="Z28" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="AA28" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="AC28" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="AD28" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="AE28" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="AF28" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="AH28" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="AI28" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="AI28" s="3" t="s">
-        <v>235</v>
-      </c>
       <c r="AJ28" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="AK28" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="AL28" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="AN28" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="AO28" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="AQ28" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="AR28" s="3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="AS28" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="AT28" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="29" spans="1:46" x14ac:dyDescent="0.25">
@@ -2416,55 +2605,52 @@
         <v>214</v>
       </c>
       <c r="Z29" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="AA29" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AC29" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AD29" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="AE29" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="AF29" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="AH29" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="AI29" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="AJ29" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AK29" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="AL29" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="AN29" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="AO29" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="AQ29" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="AR29" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="AS29" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="AT29" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="30" spans="1:46" x14ac:dyDescent="0.25">
@@ -2538,89 +2724,352 @@
         <v>215</v>
       </c>
       <c r="Z30" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="AA30" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="AC30" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="AD30" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="AE30" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AF30" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="AH30" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="AI30" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AJ30" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="AK30" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="AL30" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="AN30" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="AO30" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="AQ30" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="AR30" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="AS30" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="AT30" s="3" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="33" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A33" s="9">
+        <v>2</v>
+      </c>
+      <c r="B33" s="9"/>
+      <c r="D33" s="13">
+        <v>5</v>
+      </c>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="13"/>
+      <c r="J33" s="13">
+        <v>2</v>
+      </c>
+      <c r="K33" s="13"/>
+      <c r="M33" s="13">
+        <v>3</v>
+      </c>
+      <c r="N33" s="13"/>
+      <c r="O33" s="13"/>
+      <c r="Q33" s="13">
+        <v>3</v>
+      </c>
+      <c r="R33" s="13"/>
+      <c r="S33" s="13"/>
+      <c r="U33" s="13">
+        <v>3</v>
+      </c>
+      <c r="V33" s="13"/>
+      <c r="W33" s="13"/>
+      <c r="Y33" s="13">
+        <v>6</v>
+      </c>
+      <c r="Z33" s="13"/>
+      <c r="AA33" s="13"/>
+      <c r="AB33" s="13"/>
+      <c r="AC33" s="13"/>
+      <c r="AD33" s="13"/>
+    </row>
+    <row r="34" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="12">
-        <v>2</v>
-      </c>
-      <c r="B33" s="12"/>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
+      <c r="B34" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="J34" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="K34" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="M34" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="N34" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="O34" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="Q34" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="R34" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="S34" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="U34" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="V34" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="W34" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="Y34" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="Z34" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="AA34" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="AB34" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="AC34" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="AD34" s="3" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="35" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B35" s="3" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
+      <c r="D35" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="J35" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="K35" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="M35" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="N35" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="O35" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="Q35" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="R35" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="S35" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="U35" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="V35" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="W35" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="Y35" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="Z35" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="AA35" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="AB35" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="AC35" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="AD35" s="3" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="36" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B36" s="3" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
-        <v>267</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>270</v>
-      </c>
+      <c r="D36" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="J36" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="K36" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="M36" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="N36" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="O36" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="Q36" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="R36" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="S36" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="U36" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="V36" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="W36" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="Y36" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="Z36" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="AA36" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="AB36" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="AC36" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="AD36" s="3" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="39" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A39" s="7" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="40" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A40" s="11">
+        <f>SUM(A27,A33,D33,J33,M33,I27,Q33,T27,U33,AN27,AQ27,AH27,AC27,Y33)</f>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="41" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A41" s="11"/>
+    </row>
+    <row r="42" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A42" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="25">
+  <mergeCells count="32">
+    <mergeCell ref="A40:A42"/>
+    <mergeCell ref="T27:Z27"/>
+    <mergeCell ref="AB11:AG11"/>
+    <mergeCell ref="AI11:AL11"/>
+    <mergeCell ref="AN11:AR11"/>
+    <mergeCell ref="D33:H33"/>
+    <mergeCell ref="J33:K33"/>
+    <mergeCell ref="M33:O33"/>
+    <mergeCell ref="Q33:S33"/>
+    <mergeCell ref="U33:W33"/>
+    <mergeCell ref="Y33:AD33"/>
+    <mergeCell ref="O17:Q17"/>
+    <mergeCell ref="S17:V17"/>
+    <mergeCell ref="X17:Y17"/>
+    <mergeCell ref="A11:G11"/>
+    <mergeCell ref="I11:Q11"/>
+    <mergeCell ref="S11:Z11"/>
     <mergeCell ref="AH27:AL27"/>
     <mergeCell ref="AN27:AO27"/>
     <mergeCell ref="AQ27:AT27"/>
@@ -2632,20 +3081,10 @@
     <mergeCell ref="A23:A25"/>
     <mergeCell ref="A27:G27"/>
     <mergeCell ref="I27:R27"/>
-    <mergeCell ref="T27:AA27"/>
     <mergeCell ref="AC27:AF27"/>
     <mergeCell ref="A17:E17"/>
     <mergeCell ref="G17:I17"/>
     <mergeCell ref="K17:M17"/>
-    <mergeCell ref="O17:Q17"/>
-    <mergeCell ref="S17:V17"/>
-    <mergeCell ref="X17:Y17"/>
-    <mergeCell ref="A11:G11"/>
-    <mergeCell ref="I11:Q11"/>
-    <mergeCell ref="S11:Z11"/>
-    <mergeCell ref="AB11:AG11"/>
-    <mergeCell ref="AI11:AL11"/>
-    <mergeCell ref="AN11:AR11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
Finish game 1.0 Version, at the future i'll we adding more options
</commit_message>
<xml_diff>
--- a/Verbs list.xlsx
+++ b/Verbs list.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="359">
   <si>
     <t>catch</t>
   </si>
@@ -437,9 +437,6 @@
     <t>shod</t>
   </si>
   <si>
-    <t>sid</t>
-  </si>
-  <si>
     <t>sat</t>
   </si>
   <si>
@@ -1020,6 +1017,90 @@
   </si>
   <si>
     <t>Group B</t>
+  </si>
+  <si>
+    <t>lead</t>
+  </si>
+  <si>
+    <t>led</t>
+  </si>
+  <si>
+    <t>sit</t>
+  </si>
+  <si>
+    <t>let</t>
+  </si>
+  <si>
+    <t>set</t>
+  </si>
+  <si>
+    <t>upset</t>
+  </si>
+  <si>
+    <t>wet</t>
+  </si>
+  <si>
+    <t>bet</t>
+  </si>
+  <si>
+    <t>spread</t>
+  </si>
+  <si>
+    <t>sweat</t>
+  </si>
+  <si>
+    <t>Beat</t>
+  </si>
+  <si>
+    <t>Spread</t>
+  </si>
+  <si>
+    <t>Sweat</t>
+  </si>
+  <si>
+    <t>Bet</t>
+  </si>
+  <si>
+    <t>Wet</t>
+  </si>
+  <si>
+    <t>Upset</t>
+  </si>
+  <si>
+    <t>Set</t>
+  </si>
+  <si>
+    <t>Let</t>
+  </si>
+  <si>
+    <t>cut</t>
+  </si>
+  <si>
+    <t>Shut</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>Hurt</t>
+  </si>
+  <si>
+    <t>Burst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Put </t>
+  </si>
+  <si>
+    <t>Cast</t>
+  </si>
+  <si>
+    <t>Broadcast</t>
+  </si>
+  <si>
+    <t>Forecast</t>
+  </si>
+  <si>
+    <t>Group C</t>
   </si>
 </sst>
 </file>
@@ -1065,7 +1146,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1102,8 +1183,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1135,11 +1222,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1162,22 +1275,43 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1460,15 +1594,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AT42"/>
+  <dimension ref="A1:AT59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:A25"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="46.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="18" style="1" customWidth="1"/>
     <col min="2" max="2" width="18.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="19.42578125" style="1" customWidth="1"/>
     <col min="4" max="5" width="11.42578125" style="1"/>
@@ -1482,57 +1616,58 @@
     <col min="37" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
     </row>
-    <row r="2" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="6"/>
     </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="6"/>
     </row>
-    <row r="4" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="6"/>
     </row>
-    <row r="5" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="6"/>
     </row>
-    <row r="6" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="6"/>
     </row>
-    <row r="7" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="6"/>
     </row>
-    <row r="8" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="6"/>
     </row>
-    <row r="9" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
     </row>
-    <row r="10" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
-    </row>
-    <row r="11" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="AA10" s="16"/>
+    </row>
+    <row r="11" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>7</v>
       </c>
@@ -1563,6 +1698,7 @@
       <c r="X11" s="10"/>
       <c r="Y11" s="10"/>
       <c r="Z11" s="10"/>
+      <c r="AA11" s="16"/>
       <c r="AB11" s="10">
         <v>6</v>
       </c>
@@ -1578,14 +1714,15 @@
       <c r="AK11" s="10"/>
       <c r="AL11" s="10"/>
       <c r="AN11" s="10">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AO11" s="10"/>
       <c r="AP11" s="10"/>
       <c r="AQ11" s="10"/>
       <c r="AR11" s="10"/>
-    </row>
-    <row r="12" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="AS11" s="10"/>
+    </row>
+    <row r="12" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>1</v>
       </c>
@@ -1657,11 +1794,11 @@
       <c r="Y12" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="Z12" s="3" t="s">
+      <c r="Z12" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="AA12" s="3"/>
-      <c r="AB12" s="3" t="s">
+      <c r="AA12" s="16"/>
+      <c r="AB12" s="15" t="s">
         <v>50</v>
       </c>
       <c r="AC12" s="3" t="s">
@@ -1708,8 +1845,11 @@
       <c r="AR12" s="3" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="13" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="AS12" s="3" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="13" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>2</v>
       </c>
@@ -1781,11 +1921,11 @@
       <c r="Y13" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="Z13" s="3" t="s">
+      <c r="Z13" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="AA13" s="3"/>
-      <c r="AB13" s="3" t="s">
+      <c r="AA13" s="16"/>
+      <c r="AB13" s="15" t="s">
         <v>51</v>
       </c>
       <c r="AC13" s="3" t="s">
@@ -1832,8 +1972,11 @@
       <c r="AR13" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="14" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="AS13" s="3" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="14" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>2</v>
       </c>
@@ -1905,11 +2048,11 @@
       <c r="Y14" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="Z14" s="3" t="s">
+      <c r="Z14" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="AA14" s="3"/>
-      <c r="AB14" s="3" t="s">
+      <c r="AA14" s="16"/>
+      <c r="AB14" s="15" t="s">
         <v>51</v>
       </c>
       <c r="AC14" s="3" t="s">
@@ -1956,6 +2099,15 @@
       <c r="AR14" s="3" t="s">
         <v>79</v>
       </c>
+      <c r="AS14" s="3" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="15" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AA15" s="16"/>
+    </row>
+    <row r="16" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AA16" s="16"/>
     </row>
     <row r="17" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
@@ -2103,23 +2255,23 @@
       </c>
       <c r="AI18" s="3"/>
       <c r="AJ18" s="3" t="s">
-        <v>137</v>
+        <v>333</v>
       </c>
       <c r="AK18" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AL18" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AM18" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AN18" s="3"/>
       <c r="AO18" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="AP18" s="3" t="s">
         <v>145</v>
-      </c>
-      <c r="AP18" s="3" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="19" spans="1:46" x14ac:dyDescent="0.25">
@@ -2213,23 +2365,23 @@
       </c>
       <c r="AI19" s="3"/>
       <c r="AJ19" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AK19" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AL19" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AM19" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AN19" s="3"/>
       <c r="AO19" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AP19" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="20" spans="1:46" x14ac:dyDescent="0.25">
@@ -2323,752 +2475,956 @@
       </c>
       <c r="AI20" s="3"/>
       <c r="AJ20" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AK20" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AL20" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AM20" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AN20" s="3"/>
       <c r="AO20" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AP20" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="22" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="23" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A23" s="11">
+      <c r="A23" s="8">
         <f>SUM(A11,A17,G17,I11,K17,O17,S17,S11,X17,AB11,AI11:AL11,AF17,AJ17,AN11,AO17,AA17)</f>
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A24" s="11"/>
+      <c r="A24" s="8"/>
     </row>
     <row r="25" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A25" s="11"/>
+      <c r="A25" s="8"/>
     </row>
     <row r="27" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A27" s="12">
+      <c r="A27" s="13">
         <v>7</v>
       </c>
-      <c r="B27" s="12"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="12"/>
-      <c r="I27" s="8">
+      <c r="B27" s="13"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
+      <c r="I27" s="9">
         <v>10</v>
       </c>
-      <c r="J27" s="8"/>
-      <c r="K27" s="8"/>
-      <c r="L27" s="8"/>
-      <c r="M27" s="8"/>
-      <c r="N27" s="8"/>
-      <c r="O27" s="8"/>
-      <c r="P27" s="8"/>
-      <c r="Q27" s="8"/>
-      <c r="R27" s="8"/>
-      <c r="T27" s="8">
+      <c r="J27" s="9"/>
+      <c r="K27" s="9"/>
+      <c r="L27" s="9"/>
+      <c r="M27" s="9"/>
+      <c r="N27" s="9"/>
+      <c r="O27" s="9"/>
+      <c r="P27" s="9"/>
+      <c r="Q27" s="9"/>
+      <c r="R27" s="9"/>
+      <c r="T27" s="9">
         <v>7</v>
       </c>
-      <c r="U27" s="8"/>
-      <c r="V27" s="8"/>
-      <c r="W27" s="8"/>
-      <c r="X27" s="8"/>
-      <c r="Y27" s="8"/>
-      <c r="Z27" s="8"/>
+      <c r="U27" s="9"/>
+      <c r="V27" s="9"/>
+      <c r="W27" s="9"/>
+      <c r="X27" s="9"/>
+      <c r="Y27" s="9"/>
+      <c r="Z27" s="9"/>
       <c r="AA27" s="6"/>
-      <c r="AC27" s="8">
+      <c r="AC27" s="9">
         <v>4</v>
       </c>
-      <c r="AD27" s="8"/>
-      <c r="AE27" s="8"/>
-      <c r="AF27" s="8"/>
-      <c r="AH27" s="8">
+      <c r="AD27" s="9"/>
+      <c r="AE27" s="9"/>
+      <c r="AF27" s="9"/>
+      <c r="AH27" s="9">
         <v>5</v>
       </c>
-      <c r="AI27" s="8"/>
-      <c r="AJ27" s="8"/>
-      <c r="AK27" s="8"/>
-      <c r="AL27" s="8"/>
-      <c r="AN27" s="8">
+      <c r="AI27" s="9"/>
+      <c r="AJ27" s="9"/>
+      <c r="AK27" s="9"/>
+      <c r="AL27" s="9"/>
+      <c r="AN27" s="9">
         <v>2</v>
       </c>
-      <c r="AO27" s="8"/>
-      <c r="AQ27" s="8">
+      <c r="AO27" s="9"/>
+      <c r="AQ27" s="9">
         <v>4</v>
       </c>
-      <c r="AR27" s="8"/>
-      <c r="AS27" s="8"/>
-      <c r="AT27" s="8"/>
+      <c r="AR27" s="9"/>
+      <c r="AS27" s="9"/>
+      <c r="AT27" s="9"/>
     </row>
     <row r="28" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="K28" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="L28" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M28" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="N28" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="O28" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="P28" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="Q28" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="R28" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="T28" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="U28" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="V28" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="V28" s="3" t="s">
-        <v>204</v>
-      </c>
       <c r="W28" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="X28" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="Y28" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="Z28" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AC28" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="AD28" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="AE28" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="AF28" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AH28" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="AI28" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="AI28" s="3" t="s">
-        <v>234</v>
-      </c>
       <c r="AJ28" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AK28" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="AL28" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="AN28" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="AO28" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="AQ28" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="AR28" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="AS28" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="AT28" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="29" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="K29" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="L29" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M29" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="N29" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="O29" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="P29" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="Q29" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="R29" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="T29" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="U29" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="V29" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="W29" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="X29" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="Y29" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="Z29" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="AC29" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="AD29" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="AE29" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="AF29" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="AH29" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="AI29" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="AJ29" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="AK29" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="AL29" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="AN29" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="AO29" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="AQ29" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="AR29" s="3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="AS29" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="AT29" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="30" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F30" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="G30" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="G30" s="3" t="s">
-        <v>167</v>
-      </c>
       <c r="I30" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="K30" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="L30" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="M30" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="N30" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="O30" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="P30" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="Q30" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="R30" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="R30" s="3" t="s">
-        <v>196</v>
-      </c>
       <c r="T30" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="U30" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="U30" s="3" t="s">
-        <v>201</v>
-      </c>
       <c r="V30" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="W30" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="X30" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="Y30" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="Z30" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AC30" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AD30" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="AE30" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="AF30" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="AH30" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="AI30" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="AJ30" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AK30" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="AL30" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="AN30" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="AO30" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="AQ30" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="AR30" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="AS30" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="AT30" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="33" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A33" s="9">
+      <c r="A33" s="12">
         <v>2</v>
       </c>
-      <c r="B33" s="9"/>
-      <c r="D33" s="13">
+      <c r="B33" s="12"/>
+      <c r="D33" s="11">
         <v>5</v>
       </c>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
-      <c r="H33" s="13"/>
-      <c r="J33" s="13">
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
+      <c r="J33" s="11">
         <v>2</v>
       </c>
-      <c r="K33" s="13"/>
-      <c r="M33" s="13">
+      <c r="K33" s="11"/>
+      <c r="M33" s="11">
         <v>3</v>
       </c>
-      <c r="N33" s="13"/>
-      <c r="O33" s="13"/>
-      <c r="Q33" s="13">
+      <c r="N33" s="11"/>
+      <c r="O33" s="11"/>
+      <c r="Q33" s="11">
         <v>3</v>
       </c>
-      <c r="R33" s="13"/>
-      <c r="S33" s="13"/>
-      <c r="U33" s="13">
+      <c r="R33" s="11"/>
+      <c r="S33" s="11"/>
+      <c r="U33" s="11">
         <v>3</v>
       </c>
-      <c r="V33" s="13"/>
-      <c r="W33" s="13"/>
-      <c r="Y33" s="13">
+      <c r="V33" s="11"/>
+      <c r="W33" s="11"/>
+      <c r="Y33" s="11">
         <v>6</v>
       </c>
-      <c r="Z33" s="13"/>
-      <c r="AA33" s="13"/>
-      <c r="AB33" s="13"/>
-      <c r="AC33" s="13"/>
-      <c r="AD33" s="13"/>
+      <c r="Z33" s="11"/>
+      <c r="AA33" s="11"/>
+      <c r="AB33" s="11"/>
+      <c r="AC33" s="11"/>
+      <c r="AD33" s="11"/>
     </row>
     <row r="34" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="K34" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="M34" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="N34" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="O34" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="Q34" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="R34" s="3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="S34" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="U34" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="V34" s="3" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="W34" s="3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="Y34" s="3" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="Z34" s="3" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="AA34" s="3" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="AB34" s="3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="AC34" s="3" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="AD34" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="35" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="K35" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="M35" s="3" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="N35" s="3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="O35" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="Q35" s="3" t="s">
         <v>94</v>
       </c>
       <c r="R35" s="3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="S35" s="3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="U35" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="V35" s="3" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="W35" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="Y35" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="Z35" s="3" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="AA35" s="3" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="AB35" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="AC35" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="AD35" s="3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="36" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F36" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="G36" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="G36" s="3" t="s">
-        <v>279</v>
-      </c>
       <c r="H36" s="3" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="K36" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="M36" s="3" t="s">
         <v>289</v>
       </c>
-      <c r="M36" s="3" t="s">
-        <v>290</v>
-      </c>
       <c r="N36" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="O36" s="3" t="s">
         <v>293</v>
       </c>
-      <c r="O36" s="3" t="s">
-        <v>294</v>
-      </c>
       <c r="Q36" s="3" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="R36" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="S36" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="U36" s="3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="V36" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="W36" s="3" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="Y36" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="Z36" s="3" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="AA36" s="3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="AB36" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="AC36" s="3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="AD36" s="3" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="38" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A38" s="7" t="s">
         <v>330</v>
       </c>
     </row>
     <row r="39" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A39" s="7" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="40" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A40" s="11">
+      <c r="A39" s="8">
         <f>SUM(A27,A33,D33,J33,M33,I27,Q33,T27,U33,AN27,AQ27,AH27,AC27,Y33)</f>
         <v>63</v>
       </c>
     </row>
+    <row r="40" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A40" s="8"/>
+    </row>
     <row r="41" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A41" s="11"/>
-    </row>
-    <row r="42" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A42" s="11"/>
+      <c r="A41" s="8"/>
+    </row>
+    <row r="44" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A44" s="20">
+        <v>8</v>
+      </c>
+      <c r="B44" s="20"/>
+      <c r="C44" s="20"/>
+      <c r="D44" s="20"/>
+      <c r="E44" s="20"/>
+      <c r="F44" s="20"/>
+      <c r="G44" s="20"/>
+      <c r="H44" s="20"/>
+      <c r="J44" s="20">
+        <v>3</v>
+      </c>
+      <c r="K44" s="20"/>
+      <c r="L44" s="20"/>
+      <c r="M44" s="17"/>
+    </row>
+    <row r="45" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="H45" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="J45" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="K45" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="L45" s="3" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="46" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="H46" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="J46" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="K46" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="L46" s="3" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="47" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="H47" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="J47" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="K47" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="L47" s="3" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C50" s="19">
+        <v>2</v>
+      </c>
+      <c r="D50" s="19"/>
+      <c r="F50" s="18">
+        <v>1</v>
+      </c>
+      <c r="H50" s="20">
+        <v>3</v>
+      </c>
+      <c r="I50" s="20"/>
+      <c r="J50" s="20"/>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C51" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="H51" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="I51" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="J51" s="3" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C52" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="F52" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="H52" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="I52" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="J52" s="3" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C53" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="H53" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="I53" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="J53" s="3" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56" s="7" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57" s="8">
+        <f>SUM(A44,C50,F50,H50,J44)</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58" s="8"/>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="32">
-    <mergeCell ref="A40:A42"/>
-    <mergeCell ref="T27:Z27"/>
-    <mergeCell ref="AB11:AG11"/>
-    <mergeCell ref="AI11:AL11"/>
-    <mergeCell ref="AN11:AR11"/>
-    <mergeCell ref="D33:H33"/>
-    <mergeCell ref="J33:K33"/>
-    <mergeCell ref="M33:O33"/>
-    <mergeCell ref="Q33:S33"/>
-    <mergeCell ref="U33:W33"/>
-    <mergeCell ref="Y33:AD33"/>
-    <mergeCell ref="O17:Q17"/>
-    <mergeCell ref="S17:V17"/>
-    <mergeCell ref="X17:Y17"/>
-    <mergeCell ref="A11:G11"/>
-    <mergeCell ref="I11:Q11"/>
+  <mergeCells count="37">
+    <mergeCell ref="A57:A59"/>
+    <mergeCell ref="AN11:AS11"/>
+    <mergeCell ref="J44:L44"/>
+    <mergeCell ref="H50:J50"/>
+    <mergeCell ref="A44:H44"/>
+    <mergeCell ref="C50:D50"/>
     <mergeCell ref="S11:Z11"/>
     <mergeCell ref="AH27:AL27"/>
     <mergeCell ref="AN27:AO27"/>
@@ -3085,6 +3441,21 @@
     <mergeCell ref="A17:E17"/>
     <mergeCell ref="G17:I17"/>
     <mergeCell ref="K17:M17"/>
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="T27:Z27"/>
+    <mergeCell ref="AB11:AG11"/>
+    <mergeCell ref="AI11:AL11"/>
+    <mergeCell ref="D33:H33"/>
+    <mergeCell ref="J33:K33"/>
+    <mergeCell ref="M33:O33"/>
+    <mergeCell ref="Q33:S33"/>
+    <mergeCell ref="U33:W33"/>
+    <mergeCell ref="Y33:AD33"/>
+    <mergeCell ref="O17:Q17"/>
+    <mergeCell ref="S17:V17"/>
+    <mergeCell ref="X17:Y17"/>
+    <mergeCell ref="A11:G11"/>
+    <mergeCell ref="I11:Q11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>